<commit_message>
Output Always change according to the date and face
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Current_Date</t>
   </si>
@@ -31,13 +31,7 @@
     <t>anand</t>
   </si>
   <si>
-    <t>vipin</t>
-  </si>
-  <si>
-    <t>15:21:08</t>
-  </si>
-  <si>
-    <t>15:21:46</t>
+    <t>15:49:41</t>
   </si>
 </sst>
 </file>
@@ -395,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,18 +414,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>